<commit_message>
updated manual test cases
</commit_message>
<xml_diff>
--- a/TestCases/ComputerDatabasesTestcases.xlsx
+++ b/TestCases/ComputerDatabasesTestcases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RC08508\OneDrive - Ryan LLC\Desktop\TestCases Heroku\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RC08508\CypressComputers\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B5553C-27E9-4050-95DD-F19CCBC8F76E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F2656A-CAD8-415C-9260-12720DC92C30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{45FA9105-9813-40E2-862F-BA5375CCF139}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="69">
   <si>
     <t>Test Scenario</t>
   </si>
@@ -200,7 +200,58 @@
     <t>List of Computer Names should be sorted accordingly</t>
   </si>
   <si>
-    <t>Edit Computer</t>
+    <t>Edit an existing Computer</t>
+  </si>
+  <si>
+    <t>Edit Computer Name</t>
+  </si>
+  <si>
+    <t>Edit Introduced date, Discontinued date, Company with valid date formats</t>
+  </si>
+  <si>
+    <t>Edit Introduced date, Discontinued date, Company with invalid date formats</t>
+  </si>
+  <si>
+    <t>Clear Computer Name and Save</t>
+  </si>
+  <si>
+    <t>A Computer list have to exist already before using this option</t>
+  </si>
+  <si>
+    <t>Select an existing computer from the list</t>
+  </si>
+  <si>
+    <t>User should be taken to the module to edit computer and the header label should be displayed as "Edit computer"</t>
+  </si>
+  <si>
+    <t>Click on Save this Computer</t>
+  </si>
+  <si>
+    <t>Computer Name field should accept Alphabetical characters, Numerical values or combination of both and then page has to be navigated to homepage with a Success message "Done! Computer **** has been updated"</t>
+  </si>
+  <si>
+    <t>Computer Name field should accept valid characters</t>
+  </si>
+  <si>
+    <t>Edit Introduced date, Discontinued date with valid date formats</t>
+  </si>
+  <si>
+    <t>These date fields should accept valid format</t>
+  </si>
+  <si>
+    <t>Edit Introduced date, Discontinued date with invalid date formats</t>
+  </si>
+  <si>
+    <t>Computer Name field should accept invalid characters</t>
+  </si>
+  <si>
+    <t>Introduced date, Discontinued date fields should turn into red error state forcing user to enter something in the field.</t>
+  </si>
+  <si>
+    <t>Edit Computer Name and clear the field</t>
+  </si>
+  <si>
+    <t>Computer Name field should be cleared without any data in it.</t>
   </si>
 </sst>
 </file>
@@ -296,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -312,9 +363,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -639,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BFD6B4F-1417-447F-98BC-7CB64421BAFB}">
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -680,13 +728,13 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -699,9 +747,9 @@
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
       <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
@@ -712,9 +760,9 @@
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
       <c r="D4" s="3" t="s">
         <v>24</v>
       </c>
@@ -725,9 +773,9 @@
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
       <c r="D5" s="3" t="s">
         <v>26</v>
       </c>
@@ -738,11 +786,11 @@
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -755,9 +803,9 @@
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
       <c r="D7" s="3" t="s">
         <v>10</v>
       </c>
@@ -768,9 +816,9 @@
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
       <c r="D8" s="3" t="s">
         <v>24</v>
       </c>
@@ -781,9 +829,9 @@
       <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
       <c r="D9" s="3" t="s">
         <v>29</v>
       </c>
@@ -794,11 +842,11 @@
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6" t="s">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -811,9 +859,9 @@
       <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="8"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="7"/>
       <c r="D11" s="3" t="s">
         <v>10</v>
       </c>
@@ -824,9 +872,9 @@
       <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="8"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="7"/>
       <c r="D12" s="3" t="s">
         <v>24</v>
       </c>
@@ -837,9 +885,9 @@
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="9"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="8"/>
       <c r="D13" s="3" t="s">
         <v>31</v>
       </c>
@@ -850,11 +898,11 @@
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6" t="s">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="3" t="s">
@@ -867,9 +915,9 @@
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
       <c r="D15" s="3" t="s">
         <v>10</v>
       </c>
@@ -880,9 +928,9 @@
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
       <c r="D16" s="3" t="s">
         <v>24</v>
       </c>
@@ -893,9 +941,9 @@
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
       <c r="D17" s="3" t="s">
         <v>34</v>
       </c>
@@ -906,13 +954,13 @@
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="4" t="s">
         <v>40</v>
       </c>
       <c r="D18" s="3" t="s">
@@ -925,9 +973,9 @@
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
       <c r="D19" s="3" t="s">
         <v>10</v>
       </c>
@@ -938,9 +986,9 @@
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
       <c r="D20" s="3" t="s">
         <v>42</v>
       </c>
@@ -951,9 +999,9 @@
       <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
       <c r="D21" s="3" t="s">
         <v>43</v>
       </c>
@@ -963,68 +1011,106 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+    <row r="22" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
+    <row r="23" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+    <row r="24" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
+      <c r="D25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+      <c r="D26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
+      <c r="D27" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
+      <c r="D28" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
@@ -1032,137 +1118,205 @@
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
+      <c r="D29" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
+      <c r="D30" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
+    <row r="31" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
+      <c r="D32" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
+      <c r="D33" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
+      <c r="D34" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
+      <c r="B35" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
+      <c r="D36" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
+      <c r="D37" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
+      <c r="D38" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
+      <c r="B39" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
+      <c r="D40" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
+      <c r="D41" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>65</v>
+      </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
+      <c r="D42" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
     </row>
     <row r="43" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>48</v>
+      <c r="A43" s="4"/>
+      <c r="B43" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>9</v>
@@ -1173,137 +1327,75 @@
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
     </row>
-    <row r="44" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
+    <row r="44" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
       <c r="D44" s="3" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
     </row>
-    <row r="49" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A49" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-    </row>
-    <row r="50" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A50" s="6"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-    </row>
-    <row r="51" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A51" s="6"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-    </row>
-    <row r="52" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A52" s="6"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-    </row>
-    <row r="53" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A53" s="6"/>
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="6"/>
-      <c r="B54" s="6"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
-    </row>
-    <row r="55" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="6"/>
-      <c r="B55" s="6"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
+    <row r="45" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+    </row>
+    <row r="46" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G17" xr:uid="{006395C0-66A0-4396-88FD-8FBD3F747317}"/>
-  <mergeCells count="18">
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C14:C17"/>
+  <mergeCells count="27">
     <mergeCell ref="A2:A17"/>
     <mergeCell ref="C10:C13"/>
-    <mergeCell ref="A49:A55"/>
+    <mergeCell ref="A31:A46"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="C43:C46"/>
+    <mergeCell ref="A24:A30"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="C2:C5"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="C6:C9"/>
-    <mergeCell ref="C49:C55"/>
-    <mergeCell ref="B49:B55"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="C24:C30"/>
+    <mergeCell ref="B24:B30"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="A22:A23"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="C18:C21"/>
     <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C14:C17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>